<commit_message>
Actualización data, readme y archivo Tarea
</commit_message>
<xml_diff>
--- a/Datos_Proyecto.xlsx
+++ b/Datos_Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed09d7c5f0d5d8a3/26.- Comisión Regional Ciencia y Tecnologia Valparaíso (CORECYT)/Escritorio 1/Diplomado de análisis de datos en Biociencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABF33B10-F292-44CF-927B-54E4FD1D3830}"/>
+  <xr:revisionPtr revIDLastSave="265" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FD5DF54-3EEC-4BE7-B337-C988C19D5F6B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6CB8EC4-629D-46C0-9DD0-C343A5C4D173}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="39">
   <si>
     <t xml:space="preserve">Sesonal </t>
   </si>
@@ -187,6 +187,9 @@
   <si>
     <t>hora 3</t>
   </si>
+  <si>
+    <t>R3</t>
+  </si>
 </sst>
 </file>
 
@@ -196,7 +199,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="[$-580A]hh:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="167" formatCode="[$-580A]hh:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -325,13 +328,13 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A4D517-96D9-461A-81A7-283717F94253}">
   <dimension ref="A1:Y348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101:C109"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104:D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +927,7 @@
         <v>hora 1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E4" s="7">
         <v>1.5209999999999999</v>
@@ -1163,7 +1166,7 @@
         <v>hora 2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E7" s="7">
         <v>1.1659999999999999</v>
@@ -1401,7 +1404,7 @@
         <v>hora 3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E10" s="7">
         <v>1.0840000000000001</v>
@@ -1639,7 +1642,7 @@
         <v>hora 1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E13" s="7">
         <v>1.256</v>
@@ -1878,7 +1881,7 @@
         <v>hora 2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7">
         <v>1.5469999999999999</v>
@@ -2116,7 +2119,7 @@
         <v>hora 3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E19" s="7">
         <v>1.677</v>
@@ -2354,7 +2357,7 @@
         <v>hora 1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E22" s="7">
         <v>1.1659999999999999</v>
@@ -2593,7 +2596,7 @@
         <v>hora 2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E25" s="7">
         <v>1.385</v>
@@ -2831,7 +2834,7 @@
         <v>hora 3</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E28" s="7">
         <v>1.1759999999999999</v>
@@ -3068,7 +3071,7 @@
         <v>hora 1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E31" s="7">
         <v>0.88300000000000001</v>
@@ -3307,7 +3310,7 @@
         <v>hora 2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E34" s="7">
         <v>0.82599999999999996</v>
@@ -3545,7 +3548,7 @@
         <v>hora 3</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E37" s="7">
         <v>0.92900000000000005</v>
@@ -3783,7 +3786,7 @@
         <v>hora 1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E40" s="7">
         <v>0.85499999999999998</v>
@@ -4022,7 +4025,7 @@
         <v>hora 2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E43" s="7">
         <v>1.2450000000000001</v>
@@ -4260,7 +4263,7 @@
         <v>hora 3</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E46" s="7">
         <v>1.006</v>
@@ -4498,7 +4501,7 @@
         <v>hora 1</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E49" s="7">
         <v>1.1080000000000001</v>
@@ -4737,7 +4740,7 @@
         <v>hora 2</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E52" s="7">
         <v>0.80800000000000005</v>
@@ -4975,7 +4978,7 @@
         <v>hora 3</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E55" s="7">
         <v>0.82499999999999996</v>
@@ -5212,7 +5215,7 @@
         <v>hora 1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E58" s="7">
         <v>1.036</v>
@@ -5451,7 +5454,7 @@
         <v>hora 2</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E61" s="7">
         <v>1.298</v>
@@ -5689,7 +5692,7 @@
         <v>hora 3</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E64" s="7">
         <v>1.1180000000000001</v>
@@ -5927,7 +5930,7 @@
         <v>hora 1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E67" s="7">
         <v>1.0629999999999999</v>
@@ -6166,7 +6169,7 @@
         <v>hora 2</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E70" s="7">
         <v>1.526</v>
@@ -6404,7 +6407,7 @@
         <v>hora 3</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E73" s="7">
         <v>1.1399999999999999</v>
@@ -6642,7 +6645,7 @@
         <v>hora 1</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E76" s="7">
         <v>1.611</v>
@@ -6881,7 +6884,7 @@
         <v>hora 2</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E79" s="7">
         <v>1.4139999999999999</v>
@@ -7119,7 +7122,7 @@
         <v>hora 3</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E82" s="7">
         <v>1.839</v>
@@ -7356,7 +7359,7 @@
         <v>hora 1</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E85" s="7">
         <v>0.93600000000000005</v>
@@ -7595,7 +7598,7 @@
         <v>hora 2</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E88" s="7">
         <v>1.5549999999999999</v>
@@ -7833,7 +7836,7 @@
         <v>hora 3</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E91" s="7">
         <v>1.0089999999999999</v>
@@ -8071,7 +8074,7 @@
         <v>hora 1</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E94" s="7">
         <v>0.86399999999999999</v>
@@ -8310,7 +8313,7 @@
         <v>hora 2</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E97" s="7">
         <v>1.3220000000000001</v>
@@ -8548,7 +8551,7 @@
         <v>hora 3</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E100" s="7">
         <v>1.4</v>
@@ -8786,7 +8789,7 @@
         <v>hora 1</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E103" s="7">
         <v>1.31</v>
@@ -9025,7 +9028,7 @@
         <v>hora 2</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E106" s="7">
         <v>1.5580000000000001</v>
@@ -9263,7 +9266,7 @@
         <v>hora 3</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E109" s="7">
         <v>1.04</v>

</xml_diff>

<commit_message>
Actualiza set de datos y reporte de la tarea con histogramas (N°3)
</commit_message>
<xml_diff>
--- a/Datos_Proyecto.xlsx
+++ b/Datos_Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed09d7c5f0d5d8a3/26.- Comisión Regional Ciencia y Tecnologia Valparaíso (CORECYT)/Escritorio 1/Diplomado de análisis de datos en Biociencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22A7CF78-603D-4B9F-B2E2-64B73C9B680A}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{978D112A-40E0-4DB5-AF5E-AA8DA6AD1717}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6CB8EC4-629D-46C0-9DD0-C343A5C4D173}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="36">
   <si>
     <t xml:space="preserve">Sesonal </t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">pH </t>
-  </si>
-  <si>
-    <t>NO3-</t>
-  </si>
-  <si>
-    <t>PO43 -</t>
   </si>
   <si>
     <t>Temperature</t>
@@ -109,9 +103,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>C:N</t>
-  </si>
-  <si>
     <t>Autumn</t>
   </si>
   <si>
@@ -138,6 +129,21 @@
   <si>
     <t>R3</t>
   </si>
+  <si>
+    <t>Seasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrato </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfato </t>
+  </si>
+  <si>
+    <t>day 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio </t>
+  </si>
 </sst>
 </file>
 
@@ -145,8 +151,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-580A]hh:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-580A]hh:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -257,16 +263,16 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +590,7 @@
   <dimension ref="A1:T348"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +603,7 @@
     <col min="7" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" style="1" customWidth="1"/>
@@ -609,7 +615,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -618,69 +624,69 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="L1" s="4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E2" s="6">
         <v>1.04</v>
@@ -738,14 +744,14 @@
       </c>
       <c r="B3" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C3" s="16" t="str">
         <f t="shared" si="0"/>
         <v>hora 1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" s="6">
         <v>1.597</v>
@@ -803,14 +809,14 @@
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C4" s="16" t="str">
         <f t="shared" si="0"/>
         <v>hora 1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6">
         <v>1.5209999999999999</v>
@@ -868,13 +874,13 @@
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E5" s="6">
         <v>1.4790000000000001</v>
@@ -932,14 +938,14 @@
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C6" s="16" t="str">
         <f>C5</f>
         <v>hora 2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="6">
         <v>1.139</v>
@@ -997,14 +1003,14 @@
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C7" s="16" t="str">
         <f>C6</f>
         <v>hora 2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6">
         <v>1.1659999999999999</v>
@@ -1062,13 +1068,13 @@
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="6">
         <v>1.38</v>
@@ -1126,13 +1132,13 @@
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6">
         <v>1.173</v>
@@ -1190,14 +1196,14 @@
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C10" s="16" t="str">
         <f t="shared" ref="C10" si="1">C9</f>
         <v>hora 3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="6">
         <v>1.0840000000000001</v>
@@ -1254,13 +1260,13 @@
         <v>Autumn</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" s="6">
         <v>1.4910000000000001</v>
@@ -1325,7 +1331,7 @@
         <v>hora 1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="6">
         <v>1.1819999999999999</v>
@@ -1390,7 +1396,7 @@
         <v>hora 1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="6">
         <v>1.256</v>
@@ -1451,10 +1457,10 @@
         <v>day 2</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E14" s="6">
         <v>1.6990000000000001</v>
@@ -1519,7 +1525,7 @@
         <v>hora 2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="6">
         <v>1.21</v>
@@ -1584,7 +1590,7 @@
         <v>hora 2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" s="6">
         <v>1.5469999999999999</v>
@@ -1645,10 +1651,10 @@
         <v>day 2</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E17" s="6">
         <v>1.635</v>
@@ -1709,10 +1715,10 @@
         <v>day 2</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E18" s="6">
         <v>0.95299999999999996</v>
@@ -1777,7 +1783,7 @@
         <v>hora 3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E19" s="6">
         <v>1.677</v>
@@ -1834,13 +1840,13 @@
         <v>Autumn</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E20" s="6">
         <v>0.76900000000000002</v>
@@ -1905,7 +1911,7 @@
         <v>hora 1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E21" s="6">
         <v>0.96699999999999997</v>
@@ -1970,7 +1976,7 @@
         <v>hora 1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E22" s="6">
         <v>1.1659999999999999</v>
@@ -2031,10 +2037,10 @@
         <v>day 3</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E23" s="6">
         <v>1.5309999999999999</v>
@@ -2099,7 +2105,7 @@
         <v>hora 2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E24" s="6">
         <v>1.222</v>
@@ -2164,7 +2170,7 @@
         <v>hora 2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E25" s="6">
         <v>1.385</v>
@@ -2225,10 +2231,10 @@
         <v>day 3</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E26" s="6">
         <v>1.0049999999999999</v>
@@ -2289,10 +2295,10 @@
         <v>day 3</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E27" s="10">
         <v>1</v>
@@ -2357,7 +2363,7 @@
         <v>hora 3</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E28" s="6">
         <v>1.1759999999999999</v>
@@ -2410,16 +2416,16 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>30</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E29" s="6">
         <v>0.80800000000000005</v>
@@ -2477,14 +2483,14 @@
       </c>
       <c r="B30" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C30" s="16" t="str">
         <f t="shared" si="7"/>
         <v>hora 1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E30" s="6">
         <v>0.86899999999999999</v>
@@ -2542,14 +2548,14 @@
       </c>
       <c r="B31" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C31" s="16" t="str">
         <f t="shared" si="7"/>
         <v>hora 1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E31" s="6">
         <v>0.88300000000000001</v>
@@ -2607,13 +2613,13 @@
       </c>
       <c r="B32" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E32" s="6">
         <v>0.95399999999999996</v>
@@ -2671,14 +2677,14 @@
       </c>
       <c r="B33" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C33" s="16" t="str">
         <f>C32</f>
         <v>hora 2</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E33" s="6">
         <v>0.88200000000000001</v>
@@ -2736,14 +2742,14 @@
       </c>
       <c r="B34" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C34" s="16" t="str">
         <f>C33</f>
         <v>hora 2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E34" s="6">
         <v>0.82599999999999996</v>
@@ -2801,13 +2807,13 @@
       </c>
       <c r="B35" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E35" s="6">
         <v>0.81599999999999995</v>
@@ -2865,13 +2871,13 @@
       </c>
       <c r="B36" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E36" s="10">
         <v>0.87</v>
@@ -2929,14 +2935,14 @@
       </c>
       <c r="B37" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C37" s="16" t="str">
         <f t="shared" si="7"/>
         <v>hora 3</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E37" s="6">
         <v>0.92900000000000005</v>
@@ -2993,13 +2999,13 @@
         <v>Winter</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E38" s="6">
         <v>0.78600000000000003</v>
@@ -3064,7 +3070,7 @@
         <v>hora 1</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E39" s="6">
         <v>0.83499999999999996</v>
@@ -3129,7 +3135,7 @@
         <v>hora 1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E40" s="6">
         <v>0.85499999999999998</v>
@@ -3190,10 +3196,10 @@
         <v>day 2</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E41" s="6">
         <v>1.034</v>
@@ -3258,7 +3264,7 @@
         <v>hora 2</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E42" s="6">
         <v>1.0580000000000001</v>
@@ -3323,7 +3329,7 @@
         <v>hora 2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E43" s="6">
         <v>1.2450000000000001</v>
@@ -3384,10 +3390,10 @@
         <v>day 2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E44" s="6">
         <v>0.90300000000000002</v>
@@ -3448,10 +3454,10 @@
         <v>day 2</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E45" s="6">
         <v>0.91900000000000004</v>
@@ -3516,7 +3522,7 @@
         <v>hora 3</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E46" s="6">
         <v>1.006</v>
@@ -3573,13 +3579,13 @@
         <v>Winter</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E47" s="6">
         <v>0.996</v>
@@ -3644,7 +3650,7 @@
         <v>hora 1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E48" s="6">
         <v>0.81499999999999995</v>
@@ -3709,7 +3715,7 @@
         <v>hora 1</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E49" s="6">
         <v>1.1080000000000001</v>
@@ -3770,10 +3776,10 @@
         <v>day 3</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E50" s="6">
         <v>1.0209999999999999</v>
@@ -3838,7 +3844,7 @@
         <v>hora 2</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E51" s="6">
         <v>1.0129999999999999</v>
@@ -3903,7 +3909,7 @@
         <v>hora 2</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E52" s="6">
         <v>0.80800000000000005</v>
@@ -3964,10 +3970,10 @@
         <v>day 3</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E53" s="6">
         <v>0.745</v>
@@ -4028,10 +4034,10 @@
         <v>day 3</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E54" s="6">
         <v>1.038</v>
@@ -4096,7 +4102,7 @@
         <v>hora 3</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E55" s="6">
         <v>0.82499999999999996</v>
@@ -4149,16 +4155,16 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="16" t="s">
-        <v>30</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E56" s="6">
         <v>1.6160000000000001</v>
@@ -4216,14 +4222,14 @@
       </c>
       <c r="B57" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C57" s="16" t="str">
         <f t="shared" si="13"/>
         <v>hora 1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E57" s="6">
         <v>1.319</v>
@@ -4281,14 +4287,14 @@
       </c>
       <c r="B58" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C58" s="16" t="str">
         <f t="shared" si="13"/>
         <v>hora 1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E58" s="6">
         <v>1.036</v>
@@ -4346,13 +4352,13 @@
       </c>
       <c r="B59" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E59" s="6">
         <v>1.1839999999999999</v>
@@ -4410,14 +4416,14 @@
       </c>
       <c r="B60" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C60" s="16" t="str">
         <f>C59</f>
         <v>hora 2</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E60" s="6">
         <v>0.91300000000000003</v>
@@ -4475,14 +4481,14 @@
       </c>
       <c r="B61" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C61" s="16" t="str">
         <f>C60</f>
         <v>hora 2</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E61" s="6">
         <v>1.298</v>
@@ -4540,13 +4546,13 @@
       </c>
       <c r="B62" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E62" s="6">
         <v>1.0209999999999999</v>
@@ -4604,13 +4610,13 @@
       </c>
       <c r="B63" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E63" s="6">
         <v>1.0649999999999999</v>
@@ -4668,14 +4674,14 @@
       </c>
       <c r="B64" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C64" s="16" t="str">
         <f t="shared" si="13"/>
         <v>hora 3</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E64" s="6">
         <v>1.1180000000000001</v>
@@ -4732,13 +4738,13 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E65" s="6">
         <v>1.0580000000000001</v>
@@ -4803,7 +4809,7 @@
         <v>hora 1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E66" s="6">
         <v>1.2889999999999999</v>
@@ -4868,7 +4874,7 @@
         <v>hora 1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E67" s="6">
         <v>1.0629999999999999</v>
@@ -4929,10 +4935,10 @@
         <v>day 2</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E68" s="6">
         <v>1.591</v>
@@ -4997,7 +5003,7 @@
         <v>hora 2</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E69" s="6">
         <v>1.202</v>
@@ -5062,7 +5068,7 @@
         <v>hora 2</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E70" s="6">
         <v>1.526</v>
@@ -5123,10 +5129,10 @@
         <v>day 2</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E71" s="6">
         <v>1.1910000000000001</v>
@@ -5187,10 +5193,10 @@
         <v>day 2</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E72" s="6">
         <v>1.1879999999999999</v>
@@ -5255,7 +5261,7 @@
         <v>hora 3</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E73" s="6">
         <v>1.1399999999999999</v>
@@ -5312,13 +5318,13 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E74" s="6">
         <v>1.1359999999999999</v>
@@ -5383,7 +5389,7 @@
         <v>hora 1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E75" s="6">
         <v>1.9690000000000001</v>
@@ -5448,7 +5454,7 @@
         <v>hora 1</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E76" s="6">
         <v>1.611</v>
@@ -5509,10 +5515,10 @@
         <v>day 3</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E77" s="6">
         <v>1.319</v>
@@ -5577,7 +5583,7 @@
         <v>hora 2</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E78" s="6">
         <v>1.0740000000000001</v>
@@ -5642,7 +5648,7 @@
         <v>hora 2</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E79" s="6">
         <v>1.4139999999999999</v>
@@ -5703,10 +5709,10 @@
         <v>day 3</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E80" s="6">
         <v>1.635</v>
@@ -5767,10 +5773,10 @@
         <v>day 3</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E81" s="6">
         <v>1.278</v>
@@ -5835,7 +5841,7 @@
         <v>hora 3</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E82" s="6">
         <v>1.839</v>
@@ -5888,16 +5894,16 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C83" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="16" t="s">
-        <v>30</v>
-      </c>
       <c r="D83" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E83" s="6">
         <v>1.1919999999999999</v>
@@ -5955,14 +5961,14 @@
       </c>
       <c r="B84" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C84" s="16" t="str">
         <f t="shared" si="19"/>
         <v>hora 1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E84" s="6">
         <v>1.137</v>
@@ -6020,14 +6026,14 @@
       </c>
       <c r="B85" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C85" s="16" t="str">
         <f t="shared" si="19"/>
         <v>hora 1</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E85" s="6">
         <v>0.93600000000000005</v>
@@ -6085,13 +6091,13 @@
       </c>
       <c r="B86" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E86" s="6">
         <v>0.67300000000000004</v>
@@ -6149,14 +6155,14 @@
       </c>
       <c r="B87" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C87" s="16" t="str">
         <f>C86</f>
         <v>hora 2</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E87" s="6">
         <v>1.329</v>
@@ -6214,14 +6220,14 @@
       </c>
       <c r="B88" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C88" s="16" t="str">
         <f>C87</f>
         <v>hora 2</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E88" s="6">
         <v>1.5549999999999999</v>
@@ -6279,13 +6285,13 @@
       </c>
       <c r="B89" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E89" s="6">
         <v>1.1990000000000001</v>
@@ -6343,13 +6349,13 @@
       </c>
       <c r="B90" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E90" s="6">
         <v>1.21</v>
@@ -6407,14 +6413,14 @@
       </c>
       <c r="B91" s="3" t="str">
         <f t="shared" si="19"/>
-        <v>day1</v>
+        <v>day 1</v>
       </c>
       <c r="C91" s="16" t="str">
         <f t="shared" si="19"/>
         <v>hora 3</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E91" s="6">
         <v>1.0089999999999999</v>
@@ -6471,13 +6477,13 @@
         <v>Summer</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E92" s="6">
         <v>1.127</v>
@@ -6542,7 +6548,7 @@
         <v>hora 1</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E93" s="6">
         <v>1.19</v>
@@ -6607,7 +6613,7 @@
         <v>hora 1</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E94" s="6">
         <v>0.86399999999999999</v>
@@ -6668,10 +6674,10 @@
         <v>day 2</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E95" s="6">
         <v>0.94299999999999995</v>
@@ -6736,7 +6742,7 @@
         <v>hora 2</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E96" s="6">
         <v>1.4319999999999999</v>
@@ -6801,7 +6807,7 @@
         <v>hora 2</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E97" s="6">
         <v>1.3220000000000001</v>
@@ -6862,10 +6868,10 @@
         <v>day 2</v>
       </c>
       <c r="C98" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E98" s="6">
         <v>1.345</v>
@@ -6926,10 +6932,10 @@
         <v>day 2</v>
       </c>
       <c r="C99" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E99" s="6">
         <v>1.21</v>
@@ -6994,7 +7000,7 @@
         <v>hora 3</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E100" s="6">
         <v>1.4</v>
@@ -7051,13 +7057,13 @@
         <v>Summer</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C101" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E101" s="6">
         <v>1.5009999999999999</v>
@@ -7122,7 +7128,7 @@
         <v>hora 1</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E102" s="6">
         <v>1.5129999999999999</v>
@@ -7187,7 +7193,7 @@
         <v>hora 1</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E103" s="6">
         <v>1.31</v>
@@ -7248,10 +7254,10 @@
         <v>day 3</v>
       </c>
       <c r="C104" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E104" s="6">
         <v>1.5469999999999999</v>
@@ -7316,7 +7322,7 @@
         <v>hora 2</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E105" s="6">
         <v>1.5780000000000001</v>
@@ -7381,7 +7387,7 @@
         <v>hora 2</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E106" s="6">
         <v>1.5580000000000001</v>
@@ -7442,10 +7448,10 @@
         <v>day 3</v>
       </c>
       <c r="C107" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E107" s="6">
         <v>1.7070000000000001</v>
@@ -7506,10 +7512,10 @@
         <v>day 3</v>
       </c>
       <c r="C108" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E108" s="6">
         <v>0.83199999999999996</v>
@@ -7574,7 +7580,7 @@
         <v>hora 3</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E109" s="6">
         <v>1.04</v>
@@ -10473,7 +10479,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -10485,7 +10491,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" s="4"/>
     </row>
@@ -10494,16 +10500,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10512,7 +10518,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" ref="B3:D18" si="0">C2</f>
@@ -10523,7 +10529,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -10544,7 +10550,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -10564,7 +10570,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -10585,7 +10591,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -10606,7 +10612,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -10626,7 +10632,7 @@
         <v>0.75</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -10646,7 +10652,7 @@
         <v>0.75</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -10667,7 +10673,7 @@
         <v>0.75</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -10680,13 +10686,13 @@
         <v>Autumn</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -10707,7 +10713,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -10728,7 +10734,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -10748,7 +10754,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -10769,7 +10775,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -10790,7 +10796,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -10810,7 +10816,7 @@
         <v>0.75</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -10830,7 +10836,7 @@
         <v>0.75</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -10851,7 +10857,7 @@
         <v>0.75</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -10864,13 +10870,13 @@
         <v>Autumn</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D20" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -10891,7 +10897,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -10912,7 +10918,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -10932,7 +10938,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -10953,7 +10959,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -10974,7 +10980,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -10994,7 +11000,7 @@
         <v>0.75</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -11014,7 +11020,7 @@
         <v>0.75</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -11035,7 +11041,7 @@
         <v>0.75</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -11044,16 +11050,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D29" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -11074,7 +11080,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -11095,7 +11101,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -11115,7 +11121,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -11136,7 +11142,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -11157,7 +11163,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -11177,7 +11183,7 @@
         <v>0.75</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -11197,7 +11203,7 @@
         <v>0.75</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -11218,7 +11224,7 @@
         <v>0.75</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -11231,13 +11237,13 @@
         <v>Winter</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D38" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -11258,7 +11264,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -11279,7 +11285,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -11299,7 +11305,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -11320,7 +11326,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -11341,7 +11347,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -11361,7 +11367,7 @@
         <v>0.75</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -11381,7 +11387,7 @@
         <v>0.75</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -11402,7 +11408,7 @@
         <v>0.75</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -11415,13 +11421,13 @@
         <v>Winter</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D47" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -11442,7 +11448,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -11463,7 +11469,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -11483,7 +11489,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -11504,7 +11510,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -11525,7 +11531,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -11545,7 +11551,7 @@
         <v>0.75</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -11565,7 +11571,7 @@
         <v>0.75</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -11586,7 +11592,7 @@
         <v>0.75</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -11595,16 +11601,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D56" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -11625,7 +11631,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -11646,7 +11652,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -11666,7 +11672,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -11687,7 +11693,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -11708,7 +11714,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -11728,7 +11734,7 @@
         <v>0.75</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -11748,7 +11754,7 @@
         <v>0.75</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -11769,7 +11775,7 @@
         <v>0.75</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -11782,13 +11788,13 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D65" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -11809,7 +11815,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -11830,7 +11836,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -11850,7 +11856,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -11871,7 +11877,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -11892,7 +11898,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -11912,7 +11918,7 @@
         <v>0.75</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -11932,7 +11938,7 @@
         <v>0.75</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -11953,7 +11959,7 @@
         <v>0.75</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -11966,13 +11972,13 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D74" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -11993,7 +11999,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -12014,7 +12020,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -12034,7 +12040,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -12055,7 +12061,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -12076,7 +12082,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -12096,7 +12102,7 @@
         <v>0.75</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -12116,7 +12122,7 @@
         <v>0.75</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -12137,7 +12143,7 @@
         <v>0.75</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -12146,16 +12152,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D83" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -12176,7 +12182,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -12197,7 +12203,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -12217,7 +12223,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -12238,7 +12244,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -12259,7 +12265,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -12279,7 +12285,7 @@
         <v>0.75</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -12299,7 +12305,7 @@
         <v>0.75</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -12320,7 +12326,7 @@
         <v>0.75</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -12333,13 +12339,13 @@
         <v>Summer</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D92" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -12360,7 +12366,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -12381,7 +12387,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -12401,7 +12407,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -12422,7 +12428,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -12443,7 +12449,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -12463,7 +12469,7 @@
         <v>0.75</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -12483,7 +12489,7 @@
         <v>0.75</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -12504,7 +12510,7 @@
         <v>0.75</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -12517,13 +12523,13 @@
         <v>Summer</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D101" s="14">
         <v>0.41666666666666669</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -12544,7 +12550,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -12565,7 +12571,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -12585,7 +12591,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -12606,7 +12612,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -12627,7 +12633,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -12647,7 +12653,7 @@
         <v>0.75</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -12667,7 +12673,7 @@
         <v>0.75</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -12688,7 +12694,7 @@
         <v>0.75</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualiza Tarea para entrega 04/10/2022
</commit_message>
<xml_diff>
--- a/Datos_Proyecto.xlsx
+++ b/Datos_Proyecto.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed09d7c5f0d5d8a3/26.- Comisión Regional Ciencia y Tecnologia Valparaíso (CORECYT)/Escritorio 1/Diplomado de análisis de datos en Biociencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="319" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06AE30D3-DC1F-42D2-B01E-E42E31F573D4}"/>
+  <xr:revisionPtr revIDLastSave="321" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69877C7E-CB14-4654-A039-140101517C40}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F6CB8EC4-629D-46C0-9DD0-C343A5C4D173}"/>
+    <workbookView xWindow="1260" yWindow="420" windowWidth="13545" windowHeight="14940" activeTab="1" xr2:uid="{F6CB8EC4-629D-46C0-9DD0-C343A5C4D173}"/>
   </bookViews>
   <sheets>
     <sheet name="fisiologicos + ambientales" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
+    <sheet name="factores" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="31">
-  <si>
-    <t xml:space="preserve">Sesonal </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="30">
   <si>
     <t xml:space="preserve">time </t>
   </si>
@@ -570,51 +567,51 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="6">
         <v>1.04</v>
@@ -654,7 +651,7 @@
         <v>day 1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="6">
         <v>1.597</v>
@@ -694,7 +691,7 @@
         <v>day 1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6">
         <v>1.5209999999999999</v>
@@ -734,7 +731,7 @@
         <v>day 1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6">
         <v>1.4790000000000001</v>
@@ -774,7 +771,7 @@
         <v>day 1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6">
         <v>1.139</v>
@@ -814,7 +811,7 @@
         <v>day 1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="6">
         <v>1.1659999999999999</v>
@@ -854,7 +851,7 @@
         <v>day 1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="6">
         <v>1.38</v>
@@ -894,7 +891,7 @@
         <v>day 1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6">
         <v>1.173</v>
@@ -934,7 +931,7 @@
         <v>day 1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="6">
         <v>1.0840000000000001</v>
@@ -970,10 +967,10 @@
         <v>Autumn</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="6">
         <v>1.4910000000000001</v>
@@ -1013,7 +1010,7 @@
         <v>day 2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="6">
         <v>1.1819999999999999</v>
@@ -1053,7 +1050,7 @@
         <v>day 2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="6">
         <v>1.256</v>
@@ -1093,7 +1090,7 @@
         <v>day 2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="6">
         <v>1.6990000000000001</v>
@@ -1133,7 +1130,7 @@
         <v>day 2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="6">
         <v>1.21</v>
@@ -1173,7 +1170,7 @@
         <v>day 2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="6">
         <v>1.5469999999999999</v>
@@ -1213,7 +1210,7 @@
         <v>day 2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="6">
         <v>1.635</v>
@@ -1253,7 +1250,7 @@
         <v>day 2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="6">
         <v>0.95299999999999996</v>
@@ -1293,7 +1290,7 @@
         <v>day 2</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="6">
         <v>1.677</v>
@@ -1329,10 +1326,10 @@
         <v>Autumn</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="6">
         <v>0.76900000000000002</v>
@@ -1372,7 +1369,7 @@
         <v>day 3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="6">
         <v>0.96699999999999997</v>
@@ -1412,7 +1409,7 @@
         <v>day 3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="6">
         <v>1.1659999999999999</v>
@@ -1452,7 +1449,7 @@
         <v>day 3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="6">
         <v>1.5309999999999999</v>
@@ -1492,7 +1489,7 @@
         <v>day 3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="6">
         <v>1.222</v>
@@ -1532,7 +1529,7 @@
         <v>day 3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="6">
         <v>1.385</v>
@@ -1572,7 +1569,7 @@
         <v>day 3</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="6">
         <v>1.0049999999999999</v>
@@ -1612,7 +1609,7 @@
         <v>day 3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="10">
         <v>1</v>
@@ -1652,7 +1649,7 @@
         <v>day 3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="6">
         <v>1.1759999999999999</v>
@@ -1684,13 +1681,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="6">
         <v>0.80800000000000005</v>
@@ -1730,7 +1727,7 @@
         <v>day 1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="6">
         <v>0.86899999999999999</v>
@@ -1770,7 +1767,7 @@
         <v>day 1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="6">
         <v>0.88300000000000001</v>
@@ -1810,7 +1807,7 @@
         <v>day 1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="6">
         <v>0.95399999999999996</v>
@@ -1850,7 +1847,7 @@
         <v>day 1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="6">
         <v>0.88200000000000001</v>
@@ -1890,7 +1887,7 @@
         <v>day 1</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="6">
         <v>0.82599999999999996</v>
@@ -1930,7 +1927,7 @@
         <v>day 1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="6">
         <v>0.81599999999999995</v>
@@ -1970,7 +1967,7 @@
         <v>day 1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="10">
         <v>0.87</v>
@@ -2010,7 +2007,7 @@
         <v>day 1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="6">
         <v>0.92900000000000005</v>
@@ -2046,10 +2043,10 @@
         <v>Winter</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="6">
         <v>0.78600000000000003</v>
@@ -2089,7 +2086,7 @@
         <v>day 2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D39" s="6">
         <v>0.83499999999999996</v>
@@ -2129,7 +2126,7 @@
         <v>day 2</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" s="6">
         <v>0.85499999999999998</v>
@@ -2169,7 +2166,7 @@
         <v>day 2</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D41" s="6">
         <v>1.034</v>
@@ -2209,7 +2206,7 @@
         <v>day 2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D42" s="6">
         <v>1.0580000000000001</v>
@@ -2249,7 +2246,7 @@
         <v>day 2</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43" s="6">
         <v>1.2450000000000001</v>
@@ -2289,7 +2286,7 @@
         <v>day 2</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="6">
         <v>0.90300000000000002</v>
@@ -2329,7 +2326,7 @@
         <v>day 2</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D45" s="6">
         <v>0.91900000000000004</v>
@@ -2369,7 +2366,7 @@
         <v>day 2</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" s="6">
         <v>1.006</v>
@@ -2405,10 +2402,10 @@
         <v>Winter</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" s="6">
         <v>0.996</v>
@@ -2448,7 +2445,7 @@
         <v>day 3</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D48" s="6">
         <v>0.81499999999999995</v>
@@ -2488,7 +2485,7 @@
         <v>day 3</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D49" s="6">
         <v>1.1080000000000001</v>
@@ -2528,7 +2525,7 @@
         <v>day 3</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D50" s="6">
         <v>1.0209999999999999</v>
@@ -2568,7 +2565,7 @@
         <v>day 3</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D51" s="6">
         <v>1.0129999999999999</v>
@@ -2608,7 +2605,7 @@
         <v>day 3</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D52" s="6">
         <v>0.80800000000000005</v>
@@ -2648,7 +2645,7 @@
         <v>day 3</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D53" s="6">
         <v>0.745</v>
@@ -2688,7 +2685,7 @@
         <v>day 3</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D54" s="6">
         <v>1.038</v>
@@ -2728,7 +2725,7 @@
         <v>day 3</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D55" s="6">
         <v>0.82499999999999996</v>
@@ -2760,13 +2757,13 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D56" s="6">
         <v>1.6160000000000001</v>
@@ -2806,7 +2803,7 @@
         <v>day 1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D57" s="6">
         <v>1.319</v>
@@ -2846,7 +2843,7 @@
         <v>day 1</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D58" s="6">
         <v>1.036</v>
@@ -2886,7 +2883,7 @@
         <v>day 1</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D59" s="6">
         <v>1.1839999999999999</v>
@@ -2926,7 +2923,7 @@
         <v>day 1</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D60" s="6">
         <v>0.91300000000000003</v>
@@ -2966,7 +2963,7 @@
         <v>day 1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D61" s="6">
         <v>1.298</v>
@@ -3006,7 +3003,7 @@
         <v>day 1</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D62" s="6">
         <v>1.0209999999999999</v>
@@ -3046,7 +3043,7 @@
         <v>day 1</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D63" s="6">
         <v>1.0649999999999999</v>
@@ -3086,7 +3083,7 @@
         <v>day 1</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D64" s="6">
         <v>1.1180000000000001</v>
@@ -3122,10 +3119,10 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D65" s="6">
         <v>1.0580000000000001</v>
@@ -3165,7 +3162,7 @@
         <v>day 2</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66" s="6">
         <v>1.2889999999999999</v>
@@ -3205,7 +3202,7 @@
         <v>day 2</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D67" s="6">
         <v>1.0629999999999999</v>
@@ -3245,7 +3242,7 @@
         <v>day 2</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D68" s="6">
         <v>1.591</v>
@@ -3285,7 +3282,7 @@
         <v>day 2</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D69" s="6">
         <v>1.202</v>
@@ -3325,7 +3322,7 @@
         <v>day 2</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D70" s="6">
         <v>1.526</v>
@@ -3365,7 +3362,7 @@
         <v>day 2</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D71" s="6">
         <v>1.1910000000000001</v>
@@ -3405,7 +3402,7 @@
         <v>day 2</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D72" s="6">
         <v>1.1879999999999999</v>
@@ -3445,7 +3442,7 @@
         <v>day 2</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D73" s="6">
         <v>1.1399999999999999</v>
@@ -3481,10 +3478,10 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D74" s="6">
         <v>1.1359999999999999</v>
@@ -3524,7 +3521,7 @@
         <v>day 3</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D75" s="6">
         <v>1.9690000000000001</v>
@@ -3564,7 +3561,7 @@
         <v>day 3</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D76" s="6">
         <v>1.611</v>
@@ -3604,7 +3601,7 @@
         <v>day 3</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D77" s="6">
         <v>1.319</v>
@@ -3644,7 +3641,7 @@
         <v>day 3</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D78" s="6">
         <v>1.0740000000000001</v>
@@ -3684,7 +3681,7 @@
         <v>day 3</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D79" s="6">
         <v>1.4139999999999999</v>
@@ -3724,7 +3721,7 @@
         <v>day 3</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D80" s="6">
         <v>1.635</v>
@@ -3764,7 +3761,7 @@
         <v>day 3</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D81" s="6">
         <v>1.278</v>
@@ -3804,7 +3801,7 @@
         <v>day 3</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D82" s="6">
         <v>1.839</v>
@@ -3836,13 +3833,13 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D83" s="6">
         <v>1.1919999999999999</v>
@@ -3882,7 +3879,7 @@
         <v>day 1</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D84" s="6">
         <v>1.137</v>
@@ -3922,7 +3919,7 @@
         <v>day 1</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D85" s="6">
         <v>0.93600000000000005</v>
@@ -3962,7 +3959,7 @@
         <v>day 1</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D86" s="6">
         <v>0.67300000000000004</v>
@@ -4002,7 +3999,7 @@
         <v>day 1</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D87" s="6">
         <v>1.329</v>
@@ -4042,7 +4039,7 @@
         <v>day 1</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D88" s="6">
         <v>1.5549999999999999</v>
@@ -4082,7 +4079,7 @@
         <v>day 1</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D89" s="6">
         <v>1.1990000000000001</v>
@@ -4122,7 +4119,7 @@
         <v>day 1</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D90" s="6">
         <v>1.21</v>
@@ -4162,7 +4159,7 @@
         <v>day 1</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D91" s="6">
         <v>1.0089999999999999</v>
@@ -4198,10 +4195,10 @@
         <v>Summer</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D92" s="6">
         <v>1.127</v>
@@ -4241,7 +4238,7 @@
         <v>day 2</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D93" s="6">
         <v>1.19</v>
@@ -4281,7 +4278,7 @@
         <v>day 2</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D94" s="6">
         <v>0.86399999999999999</v>
@@ -4321,7 +4318,7 @@
         <v>day 2</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D95" s="6">
         <v>0.94299999999999995</v>
@@ -4361,7 +4358,7 @@
         <v>day 2</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D96" s="6">
         <v>1.4319999999999999</v>
@@ -4401,7 +4398,7 @@
         <v>day 2</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D97" s="6">
         <v>1.3220000000000001</v>
@@ -4441,7 +4438,7 @@
         <v>day 2</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D98" s="6">
         <v>1.345</v>
@@ -4481,7 +4478,7 @@
         <v>day 2</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D99" s="6">
         <v>1.21</v>
@@ -4521,7 +4518,7 @@
         <v>day 2</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D100" s="6">
         <v>1.4</v>
@@ -4557,10 +4554,10 @@
         <v>Summer</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D101" s="6">
         <v>1.5009999999999999</v>
@@ -4600,7 +4597,7 @@
         <v>day 3</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D102" s="6">
         <v>1.5129999999999999</v>
@@ -4640,7 +4637,7 @@
         <v>day 3</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D103" s="6">
         <v>1.31</v>
@@ -4680,7 +4677,7 @@
         <v>day 3</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D104" s="6">
         <v>1.5469999999999999</v>
@@ -4720,7 +4717,7 @@
         <v>day 3</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D105" s="6">
         <v>1.5780000000000001</v>
@@ -4760,7 +4757,7 @@
         <v>day 3</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D106" s="6">
         <v>1.5580000000000001</v>
@@ -4800,7 +4797,7 @@
         <v>day 3</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D107" s="6">
         <v>1.7070000000000001</v>
@@ -4840,7 +4837,7 @@
         <v>day 3</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D108" s="6">
         <v>0.83199999999999996</v>
@@ -4880,7 +4877,7 @@
         <v>day 3</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D109" s="6">
         <v>1.04</v>
@@ -6680,7 +6677,7 @@
   <dimension ref="A1:D217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,16 +6689,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6709,13 +6706,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6724,14 +6721,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" ref="B3:C18" si="0">C2</f>
         <v>day1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6748,7 +6745,7 @@
         <v>day1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6765,7 +6762,7 @@
         <v>day1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6782,7 +6779,7 @@
         <v>day1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6799,7 +6796,7 @@
         <v>day1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6816,7 +6813,7 @@
         <v>day1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6833,7 +6830,7 @@
         <v>day1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6850,7 +6847,7 @@
         <v>day1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6863,10 +6860,10 @@
         <v>Autumn</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6883,7 +6880,7 @@
         <v>day 2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6900,7 +6897,7 @@
         <v>day 2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6917,7 +6914,7 @@
         <v>day 2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6934,7 +6931,7 @@
         <v>day 2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6951,7 +6948,7 @@
         <v>day 2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -6968,7 +6965,7 @@
         <v>day 2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -6985,7 +6982,7 @@
         <v>day 2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7002,7 +6999,7 @@
         <v>day 2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7015,10 +7012,10 @@
         <v>Autumn</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7035,7 +7032,7 @@
         <v>day 3</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -7052,7 +7049,7 @@
         <v>day 3</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -7069,7 +7066,7 @@
         <v>day 3</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -7086,7 +7083,7 @@
         <v>day 3</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -7103,7 +7100,7 @@
         <v>day 3</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -7120,7 +7117,7 @@
         <v>day 3</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -7137,7 +7134,7 @@
         <v>day 3</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -7154,7 +7151,7 @@
         <v>day 3</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -7163,13 +7160,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -7186,7 +7183,7 @@
         <v>day1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -7203,7 +7200,7 @@
         <v>day1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -7220,7 +7217,7 @@
         <v>day1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -7237,7 +7234,7 @@
         <v>day1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -7254,7 +7251,7 @@
         <v>day1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -7271,7 +7268,7 @@
         <v>day1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -7288,7 +7285,7 @@
         <v>day1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -7305,7 +7302,7 @@
         <v>day1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -7318,10 +7315,10 @@
         <v>Winter</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -7338,7 +7335,7 @@
         <v>day 2</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -7355,7 +7352,7 @@
         <v>day 2</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -7372,7 +7369,7 @@
         <v>day 2</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -7389,7 +7386,7 @@
         <v>day 2</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -7406,7 +7403,7 @@
         <v>day 2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -7423,7 +7420,7 @@
         <v>day 2</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -7440,7 +7437,7 @@
         <v>day 2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -7457,7 +7454,7 @@
         <v>day 2</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -7470,10 +7467,10 @@
         <v>Winter</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -7490,7 +7487,7 @@
         <v>day 3</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -7507,7 +7504,7 @@
         <v>day 3</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -7524,7 +7521,7 @@
         <v>day 3</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -7541,7 +7538,7 @@
         <v>day 3</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -7558,7 +7555,7 @@
         <v>day 3</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -7575,7 +7572,7 @@
         <v>day 3</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -7592,7 +7589,7 @@
         <v>day 3</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -7609,7 +7606,7 @@
         <v>day 3</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -7618,13 +7615,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -7641,7 +7638,7 @@
         <v>day1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -7658,7 +7655,7 @@
         <v>day1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -7675,7 +7672,7 @@
         <v>day1</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -7692,7 +7689,7 @@
         <v>day1</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -7709,7 +7706,7 @@
         <v>day1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -7726,7 +7723,7 @@
         <v>day1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -7743,7 +7740,7 @@
         <v>day1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -7760,7 +7757,7 @@
         <v>day1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -7773,10 +7770,10 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -7793,7 +7790,7 @@
         <v>day 2</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -7810,7 +7807,7 @@
         <v>day 2</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -7827,7 +7824,7 @@
         <v>day 2</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -7844,7 +7841,7 @@
         <v>day 2</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -7861,7 +7858,7 @@
         <v>day 2</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -7878,7 +7875,7 @@
         <v>day 2</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -7895,7 +7892,7 @@
         <v>day 2</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -7912,7 +7909,7 @@
         <v>day 2</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -7925,10 +7922,10 @@
         <v xml:space="preserve">Spring </v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -7945,7 +7942,7 @@
         <v>day 3</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -7962,7 +7959,7 @@
         <v>day 3</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -7979,7 +7976,7 @@
         <v>day 3</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -7996,7 +7993,7 @@
         <v>day 3</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -8013,7 +8010,7 @@
         <v>day 3</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -8030,7 +8027,7 @@
         <v>day 3</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -8047,7 +8044,7 @@
         <v>day 3</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -8064,7 +8061,7 @@
         <v>day 3</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -8073,13 +8070,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -8096,7 +8093,7 @@
         <v>day1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -8113,7 +8110,7 @@
         <v>day1</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -8130,7 +8127,7 @@
         <v>day1</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -8147,7 +8144,7 @@
         <v>day1</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -8164,7 +8161,7 @@
         <v>day1</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -8181,7 +8178,7 @@
         <v>day1</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -8198,7 +8195,7 @@
         <v>day1</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -8215,7 +8212,7 @@
         <v>day1</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -8228,10 +8225,10 @@
         <v>Summer</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -8248,7 +8245,7 @@
         <v>day 2</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -8265,7 +8262,7 @@
         <v>day 2</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -8282,7 +8279,7 @@
         <v>day 2</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -8299,7 +8296,7 @@
         <v>day 2</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -8316,7 +8313,7 @@
         <v>day 2</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -8333,7 +8330,7 @@
         <v>day 2</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -8350,7 +8347,7 @@
         <v>day 2</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -8367,7 +8364,7 @@
         <v>day 2</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -8380,10 +8377,10 @@
         <v>Summer</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -8400,7 +8397,7 @@
         <v>day 3</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -8417,7 +8414,7 @@
         <v>day 3</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -8434,7 +8431,7 @@
         <v>day 3</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -8451,7 +8448,7 @@
         <v>day 3</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -8468,7 +8465,7 @@
         <v>day 3</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -8485,7 +8482,7 @@
         <v>day 3</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -8502,7 +8499,7 @@
         <v>day 3</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -8519,7 +8516,7 @@
         <v>day 3</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualiza tarea final 20:00 04/10/2022
</commit_message>
<xml_diff>
--- a/Datos_Proyecto.xlsx
+++ b/Datos_Proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed09d7c5f0d5d8a3/26.- Comisión Regional Ciencia y Tecnologia Valparaíso (CORECYT)/Escritorio 1/Diplomado de análisis de datos en Biociencias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="321" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69877C7E-CB14-4654-A039-140101517C40}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="8_{74ABF6CE-DBEE-4A1F-B370-F9D241DA22F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD5926AE-8CAF-410C-897D-F054A3B8AD9D}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="420" windowWidth="13545" windowHeight="14940" activeTab="1" xr2:uid="{F6CB8EC4-629D-46C0-9DD0-C343A5C4D173}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6CB8EC4-629D-46C0-9DD0-C343A5C4D173}"/>
   </bookViews>
   <sheets>
     <sheet name="fisiologicos + ambientales" sheetId="2" r:id="rId1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A4D517-96D9-461A-81A7-283717F94253}">
   <dimension ref="A1:L348"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>4.0731549101666733</v>
       </c>
       <c r="I11" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J11" s="9">
         <v>7.84</v>
@@ -1028,7 +1028,7 @@
         <v>7.8453215109932639</v>
       </c>
       <c r="I12" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J12" s="9">
         <v>7.84</v>
@@ -1068,7 +1068,7 @@
         <v>7.5833374497918644</v>
       </c>
       <c r="I13" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J13" s="9">
         <v>7.84</v>
@@ -1108,7 +1108,7 @@
         <v>7.9082612343892542</v>
       </c>
       <c r="I14" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J14" s="9">
         <v>7.85</v>
@@ -1148,7 +1148,7 @@
         <v>8.8990318072094894</v>
       </c>
       <c r="I15" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J15" s="9">
         <v>7.85</v>
@@ -1188,7 +1188,7 @@
         <v>6.8137680719853471</v>
       </c>
       <c r="I16" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J16" s="9">
         <v>7.85</v>
@@ -1228,7 +1228,7 @@
         <v>5.1903823669448421</v>
       </c>
       <c r="I17" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J17" s="9">
         <v>7.88</v>
@@ -1268,7 +1268,7 @@
         <v>8.9670730164908683</v>
       </c>
       <c r="I18" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J18" s="9">
         <v>7.88</v>
@@ -1308,7 +1308,7 @@
         <v>6.5535747429280935</v>
       </c>
       <c r="I19" s="9">
-        <v>12.29</v>
+        <v>13.29</v>
       </c>
       <c r="J19" s="9">
         <v>7.88</v>
@@ -1347,7 +1347,7 @@
         <v>7.8790301309285553</v>
       </c>
       <c r="I20" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J20" s="9">
         <v>7.84</v>
@@ -1387,7 +1387,7 @@
         <v>8.0966307095832519</v>
       </c>
       <c r="I21" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J21" s="9">
         <v>7.84</v>
@@ -1427,7 +1427,7 @@
         <v>8.6966812389657591</v>
       </c>
       <c r="I22" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J22" s="9">
         <v>7.84</v>
@@ -1467,7 +1467,7 @@
         <v>7.7915842642933075</v>
       </c>
       <c r="I23" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J23" s="9">
         <v>7.85</v>
@@ -1507,7 +1507,7 @@
         <v>6.5380163011227683</v>
       </c>
       <c r="I24" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J24" s="9">
         <v>7.85</v>
@@ -1547,7 +1547,7 @@
         <v>5.2857254449343465</v>
       </c>
       <c r="I25" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J25" s="9">
         <v>7.85</v>
@@ -1587,7 +1587,7 @@
         <v>8.2592529839482527</v>
       </c>
       <c r="I26" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J26" s="9">
         <v>7.88</v>
@@ -1627,7 +1627,7 @@
         <v>9.106008687353631</v>
       </c>
       <c r="I27" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J27" s="9">
         <v>7.88</v>
@@ -1667,7 +1667,7 @@
         <v>8.657348001745234</v>
       </c>
       <c r="I28" s="9">
-        <v>12.29</v>
+        <v>12.5</v>
       </c>
       <c r="J28" s="9">
         <v>7.88</v>
@@ -6676,7 +6676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E958556-7E38-477D-A98E-5939B3755D41}">
   <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>

</xml_diff>